<commit_message>
fixato errore in .env file per nascondere credenziali database. sostituita base di conoscenza di prova con quella di glossario Gestisco
</commit_message>
<xml_diff>
--- a/static/saved_dataframes/tabelle_entita_e_relazionali/is_Autore_documento_fonte_of.xlsx
+++ b/static/saved_dataframes/tabelle_entita_e_relazionali/is_Autore_documento_fonte_of.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -398,10 +398,720 @@
       <c r="C2" t="n">
         <v>8000001</v>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Associazione Dei Comuni Dell'Umbria Per La Protezione Civile</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Sostenibilità Dalla A Alla Z</t>
+          <t>Glossario Dei Termini Inerenti Il Mondo Della Protezione Civile</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>9000002</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8000002</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Gruppo Radio Emergenza Santena</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Piano Comunale Di Protezione Civile - Comune di Fondi</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>9000002</v>
+      </c>
+      <c r="C4" t="n">
+        <v>8000017</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Gruppo Radio Emergenza Santena</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Piano Comunale Di Protezione Civile – Comune di Fondi</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C5" t="n">
+        <v>8000003</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Glossario – Dipartimento Della Protezione Civile</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8000005</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Glossario – Conoscere Il Territorio – Città Di Gubbio</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C7" t="n">
+        <v>8000014</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Glossario Di Protezione Civile – Regione Sicilia, Comitato Regionale Della Protezione Civile</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8000015</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Benvenuti sul sito web della Centrale nazionale d'allarme CENAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8000016</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Piano Comunale Di Emergenza - Glossario</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8000019</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C11" t="n">
+        <v>8000026</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>La Protezione NBC</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C12" t="n">
+        <v>8000032</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C13" t="n">
+        <v>8000033</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Linee Guida Per La Zonazione Della Suscettibilità, Della Pericolosità E Del Rischio Da Frana Ai Fini Della Pianificazione Territoriale</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C14" t="n">
+        <v>8000035</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Le SOREU</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8000036</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Chi siamo</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C16" t="n">
+        <v>8000039</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>SOREU dei Laghi</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C17" t="n">
+        <v>8000041</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Elemento d'intervento e di supporto dello Stato maggiore federale Protezione della popolazione</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C18" t="n">
+        <v>8000042</v>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Legge sulla protezione civile del 26 febbraio 2007</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C19" t="n">
+        <v>8000044</v>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Il comando della protezione civile</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C20" t="n">
+        <v>8000045</v>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Costruzioni di protezione</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C21" t="n">
+        <v>8000046</v>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Dipartimento</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C22" t="n">
+        <v>8000048</v>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C23" t="n">
+        <v>8000053</v>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C24" t="n">
+        <v>8000060</v>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Regolamento sulla protezione della popolazione (RProtPop) (del 18 ottobre 2017)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="C25" t="n">
+        <v>8000064</v>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Segnali di allarme in Svizzera</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>9000004</v>
+      </c>
+      <c r="C26" t="n">
+        <v>8000011</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Associazione Falchi Del Sud - Napoli</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Piano Comunale Di Protezione Civile</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>9000004</v>
+      </c>
+      <c r="C27" t="n">
+        <v>8000012</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Associazione Falchi Del Sud - Napoli</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Glossario Di Protezione Civile</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>9000005</v>
+      </c>
+      <c r="C28" t="n">
+        <v>8000005</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Protezione Civile Città Di Gubbio</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Glossario – Conoscere Il Territorio – Città Di Gubbio</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>9000013</v>
+      </c>
+      <c r="C29" t="n">
+        <v>8000013</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>GEB srl</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Piano Protezione Civile Comunale – Comune Di Ravenna</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>9000015</v>
+      </c>
+      <c r="C30" t="n">
+        <v>8000006</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Regione Sicilia, Comitato Regionale Della Protezione Civile</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Acronimi Utili In Protezione E Difesa Civile</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>9000019</v>
+      </c>
+      <c r="C31" t="n">
+        <v>8000019</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Presidenza Del Consiglio Dei Ministri</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>9000034</v>
+      </c>
+      <c r="C32" t="n">
+        <v>8000032</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Alberto Bruno, Funzionario della protezione civile di regione lombardia</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>9000047</v>
+      </c>
+      <c r="C33" t="n">
+        <v>8000047</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>IRPI</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Modelli e carte di suscettibilità da frana</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>9000050</v>
+      </c>
+      <c r="C34" t="n">
+        <v>8000048</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Confederazion elvetica</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>9000058</v>
+      </c>
+      <c r="C35" t="n">
+        <v>8000053</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Ufficio Federale della Protezione della Popolazione</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>9000058</v>
+      </c>
+      <c r="C36" t="n">
+        <v>8000058</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Ufficio Federale della Protezione della Popolazione</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Il comando della protezione civile - Personale</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>9000068</v>
+      </c>
+      <c r="C37" t="n">
+        <v>8000068</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Repubblica e Cantone Ticino</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Servizio della protezione della popolazione</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>9000071</v>
+      </c>
+      <c r="C38" t="n">
+        <v>8000071</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Tommaso Sansone</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>-- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>9000071</v>
+      </c>
+      <c r="C39" t="n">
+        <v>8000076</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Tommaso Sansone</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>-- -- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>9000073</v>
+      </c>
+      <c r="C40" t="n">
+        <v>8000071</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Tommaso sansone</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>-- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
         </is>
       </c>
     </row>

</xml_diff>